<commit_message>
Commit to desktop for school
</commit_message>
<xml_diff>
--- a/EXCELSHEETS/LSI & CCPP Calculator - WQTS 2016.xlsx
+++ b/EXCELSHEETS/LSI & CCPP Calculator - WQTS 2016.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wqts/Dropbox/!WQTS Projects/Mathematical Models/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/will/Desktop/Everything/Schoolwork/Fall 2018/COMP491/AcidBaseModel/EXCELSHEETS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A6B109C1-2809-BD44-B0BD-1A4E87603FB5}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68F5E19-9EE4-F947-A202-CD322B71550C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31380" yWindow="460" windowWidth="10100" windowHeight="13920" tabRatio="698" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="698" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Portal" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
     <definedName name="Tot_Acidity">Calculations!$H$64</definedName>
     <definedName name="Tot_alk_2Ca">Calculations!$H$65</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -1683,7 +1683,7 @@
   <dimension ref="B1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="21"/>
@@ -1882,8 +1882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:V52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="21"/>

</xml_diff>

<commit_message>
Version 1.0! All calculations now functioning correctly. rounds correct!
</commit_message>
<xml_diff>
--- a/EXCELSHEETS/LSI & CCPP Calculator - WQTS 2016.xlsx
+++ b/EXCELSHEETS/LSI & CCPP Calculator - WQTS 2016.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/will/Desktop/Everything/Schoolwork/Fall 2018/COMP491/AcidBaseModel/EXCELSHEETS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CAPSTONE\AcidBaseModel\EXCELSHEETS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68F5E19-9EE4-F947-A202-CD322B71550C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CEA5C9-1FD6-4858-B5A6-32AB3D480A7D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="698" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16005" tabRatio="396" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Portal" sheetId="1" r:id="rId1"/>
     <sheet name="Calculations" sheetId="3" r:id="rId2"/>
+    <sheet name="_SSC" sheetId="4" state="veryHidden" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
     <definedName name="Alk_Blend">'[1]pH After Chem Addition'!#REF!</definedName>
@@ -32,10 +33,15 @@
     <definedName name="Tot_Acidity">Calculations!$H$64</definedName>
     <definedName name="Tot_alk_2Ca">Calculations!$H$65</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -45,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="82">
   <si>
     <t>Known Information:</t>
   </si>
@@ -812,6 +818,18 @@
   </si>
   <si>
     <t xml:space="preserve">Saturation Index (SI) = </t>
+  </si>
+  <si>
+    <t>{"BrowserAndLocation":{"ConversionPath":"C:\\Users\\chaos\\Documents\\SpreadsheetConverter","SelectedBrowsers":[]},"SpreadsheetServer":{"Username":"","Password":"","ServerUrl":"","TestUsername":"","TestPassword":""},"ConfigureSubmitDefault":{"Email":"","Free":false,"Advanced":false,"AdvancedSecured":false,"Demo":true},"MessageBubble":{"Close":false,"TopMsg":0},"CustomizeTheme":{"Theme":"C:\\Users\\user\\AppData\\Roaming\\SpreadsheetConverter\\V8\\SupportFiles\\themes\\bootstrap\\css\\default-ssc-theme.css"},"QrSetting":{"ShowOnConversion":true},"CongratsPage":{"LastOpenedVersion":""},"WordPressPluginSetting":{"IsPluginInstalled":false},"Preferences":{"IsAdvancedSettingModelInitialize":true,"IsCaptchaInitialize":true,"IsNodeSettingInitialize":false,"IsRequiredFieldModalInitialize":true,"IsSubmitDialogModelInitialize":true,"IsToolbarButtonModelInitialize":true,"IsWizardButtonModelInitialize":true,"ReadFromHidden":false,"AdvancedSetting":null,"NodeSetting":{"LoginText":{"LoginButtonText":"Login","PageDescription":"Restricted access only","LoginErrorMessage":"Authentication failed, please check your username and password.","PlaceholderPassword":"password","PlaceholderUsername":"username / email","UserExtraMessage":""}},"Captcha":{"Heading":"Enter the number displayed below.","Message":"This is to verify that you are a human visitor, to prevent automated form submissions.","OkButton":"OK","CancelButton":"Cancel","ErrorMessage":"Your answer is incorrect, please try again."},"RequiredField":{"ErrorMessage":"The fields with the red border are required or invalid.","OkButton":"OK","DDLDefaultRequiredText":"Please Select"},"WizardButton":{"Next":"Next","Previous":"Previous","Cancel":"Cancel","Finish":"Finish"},"ToolbarButton":{"Submit":"Submit","PrintSheet":"Print","PrintAll":"Print All","Reset":"Reset","Update":"Update","Back":"Back","PrintThis":"Print This"},"SubmitDialog":{"SubmitDialogHeading":"Submit Successful.","SubmitDialogDesc":"The form was successfully submitted.","BeforeSubmitDesc":"The form is being submitted.","OfflineHeading":"Save until online","OfflineDesc":"You are currently offline and the submit failed. Do you want to save the submit and send it later when you are online.","OfflineConfirm":"Do you want to save?","OfflineSubmitHeading":"Offline forms submit confirmation","OfflineSubmitDesc":"There are Offline form(s), which are now ready to submit in server.","OfflineSubmitConfirm":"Do you want to submit?","FailOfflineHeading":"Offline Form submit failed","FailOfflineDesc":"Unable to connect to the Internet. Please try submitting the offline forms later in internet connection.","OfflineSubmitWait":"It may take sometime to finish all submits depending on the size of offline forms and internet connection.","OfflineSubmitWaitCounter":"Left","OfflineSubmitError":"Submit error: Please try later."}},"UxPreferences":null}</t>
+  </si>
+  <si>
+    <t>{"InputDetection":0,"RecalcMode":0,"Name":"","Flavor":0,"Edition":0,"CopyProtect":{"IsEnabled":false,"DomainName":""},"HideSscPoweredlogo":false,"AspnetConfig":{"BrowseUrl":"http://localhost/ssc","FileExtension":0},"NodeSecureLoginEnabled":false,"SmartphoneSettings":{"ViewportLock":true,"UseOldViewEngine":false,"EnableZoom":false,"EnableSwipe":false,"HideToolbar":false,"InheritBackgroundColor":false,"CheckboxFlavor":1,"ShowBubble":false},"SmartphoneTheme":1,"Theme":{"BgColor":"#FFFFFFFF","BgImage":"","InputBorderStyle":2,"AppliedTheme":""},"Layout":0,"LayoutSamePagesHeightEnabled":false,"Toolbar":{"Position":1,"IsSubmit":true,"IsPrintSheet":false,"IsPrintAll":true,"IsPrintThis":false,"IsReset":true,"IsUpdate":true},"ConfigureSubmit":{"IsShowCaptcha":false,"IsUseSscWebServer":true,"ReceiverCode":"","IsFreeService":false,"IsAdvanceService":false,"IsSecureEmail":false,"IsDemonstrationService":true,"AfterSuccessfulSubmit":"","AfterFailSubmit":"","AfterCancelWizard":"","IsUseOwnWebServer":false,"OwnWebServerURL":"","OwnWebServerTarget":"","SubmitTarget":0},"IgnoreBgInputCell":false,"ButtonStyle":0,"ResponsiveDesignDisabled":false,"HideLookupRange":false,"BrowserStorageEnabled":false,"RealtimeSyncEnabled":true,"GoogleAnalyticsTrackingId":"","GoogleApiKey":"","ChartSelected":3,"ChartYAxisFixed":false}</t>
+  </si>
+  <si>
+    <t>{"IsHide":false,"HiddenInExcel":false,"SheetId":-1,"Name":"Calculations","Guid":"8TQNR0","Index":2,"VisibleRange":"","SheetTheme":{"TabColor":"","BodyColor":"","BodyImage":""},"IsPrintSheet":false}</t>
+  </si>
+  <si>
+    <t>{"IsHide":true,"HiddenInExcel":false,"SheetId":-1,"Name":"Portal","Guid":"HBC9SS","Index":1,"VisibleRange":"","SheetTheme":{"TabColor":"","BodyColor":"","BodyImage":""},"IsPrintSheet":false}</t>
   </si>
 </sst>
 </file>
@@ -1394,24 +1412,10 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Schematic"/>
-      <sheetName val="Raw Water Conditions"/>
       <sheetName val="pH After Chem Addition"/>
-      <sheetName val="WQ After Chem Addition"/>
-      <sheetName val="pH After Precipitation"/>
-      <sheetName val="WQ After Precipitation"/>
-      <sheetName val="pH After Acid Addition"/>
-      <sheetName val="WQ After Acid Addition"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1682,21 +1686,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="21"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="1.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="44.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="44.875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="11.875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="26">
+    <row r="1" spans="2:5" ht="26.25">
       <c r="B1" s="4" t="s">
         <v>68</v>
       </c>
@@ -1715,11 +1719,11 @@
       </c>
       <c r="C4" s="75"/>
     </row>
-    <row r="5" spans="2:5" ht="22" thickBot="1">
+    <row r="5" spans="2:5" ht="21.75" thickBot="1">
       <c r="D5" s="68"/>
       <c r="E5" s="69"/>
     </row>
-    <row r="6" spans="2:5" ht="25" thickBot="1">
+    <row r="6" spans="2:5" ht="24" thickBot="1">
       <c r="B6" s="66" t="s">
         <v>0</v>
       </c>
@@ -1727,77 +1731,77 @@
       <c r="D6" s="45"/>
       <c r="E6" s="46"/>
     </row>
-    <row r="7" spans="2:5" ht="24">
+    <row r="7" spans="2:5" ht="23.25">
       <c r="B7" s="47" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="65">
-        <v>8.08</v>
+        <v>10</v>
       </c>
       <c r="D7" s="48"/>
       <c r="E7" s="49"/>
     </row>
-    <row r="8" spans="2:5" ht="26">
+    <row r="8" spans="2:5" ht="26.25">
       <c r="B8" s="47" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="50">
-        <v>190</v>
+        <v>10</v>
       </c>
       <c r="D8" s="48" t="s">
         <v>66</v>
       </c>
       <c r="E8" s="49"/>
     </row>
-    <row r="9" spans="2:5" ht="24">
+    <row r="9" spans="2:5" ht="23.25">
       <c r="B9" s="47" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="50">
-        <v>61.2</v>
+        <v>10</v>
       </c>
       <c r="D9" s="48" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="49"/>
     </row>
-    <row r="10" spans="2:5" ht="24">
+    <row r="10" spans="2:5" ht="23.25">
       <c r="B10" s="47" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="50">
-        <v>364</v>
+        <v>10</v>
       </c>
       <c r="D10" s="48" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="49"/>
     </row>
-    <row r="11" spans="2:5" ht="28" thickBot="1">
+    <row r="11" spans="2:5" ht="28.5" thickBot="1">
       <c r="B11" s="51" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="52">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D11" s="53" t="s">
         <v>64</v>
       </c>
       <c r="E11" s="54"/>
     </row>
-    <row r="12" spans="2:5" ht="24">
+    <row r="12" spans="2:5" ht="23.25">
       <c r="B12" s="55"/>
       <c r="C12" s="55"/>
       <c r="D12" s="55"/>
       <c r="E12" s="55"/>
     </row>
-    <row r="13" spans="2:5" ht="25" thickBot="1">
+    <row r="13" spans="2:5" ht="24" thickBot="1">
       <c r="B13" s="55"/>
       <c r="C13" s="55"/>
       <c r="D13" s="55"/>
       <c r="E13" s="55"/>
     </row>
-    <row r="14" spans="2:5" ht="25" thickBot="1">
+    <row r="14" spans="2:5" ht="24" thickBot="1">
       <c r="B14" s="67" t="s">
         <v>71</v>
       </c>
@@ -1805,59 +1809,59 @@
       <c r="D14" s="56"/>
       <c r="E14" s="57"/>
     </row>
-    <row r="15" spans="2:5" ht="24">
+    <row r="15" spans="2:5" ht="23.25">
       <c r="B15" s="58" t="s">
         <v>77</v>
       </c>
       <c r="C15" s="64">
         <f>Calculations!C46</f>
-        <v>0.67259263086092791</v>
+        <v>0.28601628491065617</v>
       </c>
       <c r="D15" s="61"/>
       <c r="E15" s="62"/>
     </row>
-    <row r="16" spans="2:5" ht="32" customHeight="1">
+    <row r="16" spans="2:5" ht="32.1" customHeight="1">
       <c r="B16" s="59" t="s">
         <v>73</v>
       </c>
       <c r="C16" s="60">
         <f>Calculations!C48</f>
-        <v>18.876687058776412</v>
+        <v>2.5242952674633941</v>
       </c>
       <c r="D16" s="61" t="s">
         <v>66</v>
       </c>
       <c r="E16" s="62"/>
     </row>
-    <row r="17" spans="2:5" ht="32" customHeight="1">
+    <row r="17" spans="2:5" ht="32.1" customHeight="1">
       <c r="B17" s="59" t="s">
         <v>69</v>
       </c>
       <c r="C17" s="60">
         <f>Calculations!C49</f>
-        <v>12.543445031770428</v>
+        <v>12.397940008672037</v>
       </c>
       <c r="D17" s="61"/>
       <c r="E17" s="62"/>
     </row>
-    <row r="18" spans="2:5" ht="32" customHeight="1">
+    <row r="18" spans="2:5" ht="32.1" customHeight="1">
       <c r="B18" s="59" t="s">
         <v>70</v>
       </c>
       <c r="C18" s="60">
         <f>Calculations!C50</f>
-        <v>6.7348147382781445</v>
+        <v>9.4279674301786862</v>
       </c>
       <c r="D18" s="61"/>
       <c r="E18" s="62"/>
     </row>
-    <row r="19" spans="2:5" ht="25" thickBot="1">
+    <row r="19" spans="2:5" ht="24" thickBot="1">
       <c r="B19" s="63" t="s">
         <v>76</v>
       </c>
       <c r="C19" s="72">
         <f>Calculations!C32*12*1000</f>
-        <v>46.144559845184567</v>
+        <v>1.6309328608601348</v>
       </c>
       <c r="D19" s="73" t="s">
         <v>75</v>
@@ -1870,6 +1874,9 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <customProperties>
+    <customPr name="SSC_SHEET_GUID" r:id="rId1"/>
+  </customProperties>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1882,25 +1889,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:V52"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="21"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="1.6640625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="1.625" style="6" customWidth="1"/>
     <col min="2" max="2" width="32" style="6" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="22.125" style="6" customWidth="1"/>
     <col min="4" max="4" width="12.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="6" customWidth="1"/>
-    <col min="7" max="8" width="9.1640625" style="6"/>
+    <col min="5" max="5" width="9.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.625" style="6" customWidth="1"/>
+    <col min="7" max="8" width="9.125" style="6"/>
     <col min="9" max="9" width="14.5" style="6" customWidth="1"/>
     <col min="10" max="10" width="20" style="6" customWidth="1"/>
     <col min="11" max="20" width="19.5" style="6" customWidth="1"/>
-    <col min="21" max="21" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.1640625" style="6"/>
+    <col min="21" max="21" width="11.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.125" style="6"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:22">
@@ -1908,14 +1915,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:22" ht="22" thickBot="1"/>
+    <row r="5" spans="2:22" ht="21.75" thickBot="1"/>
     <row r="6" spans="2:22">
       <c r="B6" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="8">
         <f>Portal!C7</f>
-        <v>8.08</v>
+        <v>10</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>11</v>
@@ -1937,13 +1944,13 @@
       <c r="U6" s="12"/>
       <c r="V6" s="13"/>
     </row>
-    <row r="7" spans="2:22" ht="25">
+    <row r="7" spans="2:22" ht="24">
       <c r="B7" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="14">
         <f>Portal!C8</f>
-        <v>190</v>
+        <v>10</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>40</v>
@@ -1963,13 +1970,13 @@
       <c r="U7" s="17"/>
       <c r="V7" s="18"/>
     </row>
-    <row r="8" spans="2:22" ht="25">
+    <row r="8" spans="2:22" ht="24">
       <c r="B8" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="14">
         <f>Portal!C9*2.5</f>
-        <v>153</v>
+        <v>25</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>40</v>
@@ -1998,7 +2005,7 @@
       </c>
       <c r="C9" s="14">
         <f>Portal!C10</f>
-        <v>364</v>
+        <v>10</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>6</v>
@@ -2018,13 +2025,13 @@
       <c r="U9" s="17"/>
       <c r="V9" s="18"/>
     </row>
-    <row r="10" spans="2:22" ht="24">
+    <row r="10" spans="2:22" ht="23.25">
       <c r="B10" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="20">
         <f>Portal!C11</f>
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>41</v>
@@ -2044,7 +2051,7 @@
       <c r="U10" s="17"/>
       <c r="V10" s="18"/>
     </row>
-    <row r="11" spans="2:22" ht="22" thickBot="1">
+    <row r="11" spans="2:22" ht="21.75" thickBot="1">
       <c r="I11" s="22" t="s">
         <v>17</v>
       </c>
@@ -2094,62 +2101,62 @@
       </c>
       <c r="C12" s="28">
         <f>C9*0.000025</f>
-        <v>9.1000000000000004E-3</v>
+        <v>2.5000000000000001E-4</v>
       </c>
       <c r="I12" s="25">
         <v>1</v>
       </c>
       <c r="J12" s="26">
         <f>C6</f>
-        <v>8.08</v>
+        <v>10</v>
       </c>
       <c r="K12" s="27">
         <f>10^(-J12)/C18</f>
-        <v>9.1742788333889117E-9</v>
+        <v>1.0179280671110216E-10</v>
       </c>
       <c r="L12" s="27">
         <f t="shared" ref="L12:L48" si="0">($C$36+$C$22/$C$18^2/K12-K12)/(1+2*$C$18^2/$C$20*K12)</f>
-        <v>3.7506545272039016E-3</v>
+        <v>1.0121855789760328E-4</v>
       </c>
       <c r="M12" s="27">
         <f>$C$21/$C$19*L12/K12</f>
-        <v>2.42964149433061E-5</v>
+        <v>3.4663560539355861E-5</v>
       </c>
       <c r="N12" s="27">
         <f>$C$23/$C$19^2/M12</f>
-        <v>3.2516126163303156E-4</v>
+        <v>1.2939685585197682E-4</v>
       </c>
       <c r="O12" s="27">
         <f>$C$22/$C$18^2/K12</f>
-        <v>7.6181718831964212E-7</v>
+        <v>2.9454422816491705E-5</v>
       </c>
       <c r="P12" s="27">
         <f>$C$37-2*M12-L12-O12+K12+2*N12</f>
-        <v>-2.4096774767339369E-3</v>
+        <v>-2.4120628829604637E-4</v>
       </c>
       <c r="Q12" s="27">
         <f t="shared" ref="Q12:Q48" si="1">((-$C$22/$C$18^2/K12^2-1)*(1+2*$C$18^2*K12/$C$20)-(2*$C$18^2/$C$20)*($C$36+$C$22/$C$18^2/K12-K12))/(1+2*$C$18^2/$C$20*K12)^2</f>
-        <v>-14878.84169356026</v>
+        <v>-289760.7199623934</v>
       </c>
       <c r="R12" s="27">
         <f>$C$21/$C$19*(Q12*K12-L12)/K12^2</f>
-        <v>-2744.7026286149403</v>
+        <v>-439762.73182985373</v>
       </c>
       <c r="S12" s="27">
         <f>$C$23/$C$19^2*(-R12)/M12^2</f>
-        <v>36732.619672920788</v>
+        <v>1641606.1689638689</v>
       </c>
       <c r="T12" s="27">
         <f>-$C$22/$C$18^2/K12^2</f>
-        <v>-83.03837305958929</v>
+        <v>-289356.62320507783</v>
       </c>
       <c r="U12" s="27">
         <f>-2*R12-Q12-T12+1+2*S12</f>
-        <v>93917.524669691309</v>
+        <v>4741856.1447549164</v>
       </c>
       <c r="V12" s="18">
         <f>IF((K12-P12/U12)&lt;0,K12/10,K12-P12/U12)</f>
-        <v>3.4831657317423622E-8</v>
+        <v>1.526602900199011E-10</v>
       </c>
     </row>
     <row r="13" spans="2:22">
@@ -2158,7 +2165,7 @@
       </c>
       <c r="C13" s="32">
         <f>60954/(C10+273.15+116)-68.937</f>
-        <v>80.771952474517988</v>
+        <v>83.772507703870744</v>
       </c>
       <c r="D13" s="15"/>
       <c r="I13" s="25">
@@ -2167,55 +2174,55 @@
       </c>
       <c r="J13" s="26">
         <f>-LOG(V12*$C$18)</f>
-        <v>7.5005977964665496</v>
+        <v>9.8239910061306368</v>
       </c>
       <c r="K13" s="17">
         <f>10^(-J13)/$C$18</f>
-        <v>3.4831657317423629E-8</v>
+        <v>1.5266029001990095E-10</v>
       </c>
       <c r="L13" s="27">
         <f t="shared" si="0"/>
-        <v>3.4053679474277789E-3</v>
+        <v>9.1383587352860497E-5</v>
       </c>
       <c r="M13" s="27">
         <f>$C$21/$C$19*L13/K13</f>
-        <v>5.8102788171999309E-6</v>
+        <v>2.0867587034122788E-5</v>
       </c>
       <c r="N13" s="27">
         <f>$C$23/$C$19^2/M13</f>
-        <v>1.3597028963116635E-3</v>
+        <v>2.1494367025247455E-4</v>
       </c>
       <c r="O13" s="27">
         <f>$C$22/$C$18^2/K13</f>
-        <v>2.0065434274402499E-7</v>
+        <v>1.9640001785371708E-5</v>
       </c>
       <c r="P13" s="27">
         <f>$C$37-2*M13-L13-O13+K13+2*N13</f>
-        <v>4.2251464875721779E-5</v>
+        <v>-2.2871270041238711E-5</v>
       </c>
       <c r="Q13" s="27">
         <f t="shared" si="1"/>
-        <v>-12206.425614421967</v>
+        <v>-129055.53942050999</v>
       </c>
       <c r="R13" s="27">
         <f>$C$21/$C$19*(Q13*K13-L13)/K13^2</f>
-        <v>-187.63703567268408</v>
+        <v>-166162.99777207911</v>
       </c>
       <c r="S13" s="27">
         <f>$C$23/$C$19^2*(-R13)/M13^2</f>
-        <v>43910.219954373053</v>
+        <v>1711538.7870615784</v>
       </c>
       <c r="T13" s="27">
         <f>-$C$22/$C$18^2/K13^2</f>
-        <v>-5.7606889306312992</v>
+        <v>-128651.67348241915</v>
       </c>
       <c r="U13" s="27">
         <f>-2*R13-Q13-T13+1+2*S13</f>
-        <v>100408.90028344408</v>
+        <v>4013111.7825702438</v>
       </c>
       <c r="V13" s="18">
         <f>IF((K13-P13/U13)&lt;0,K13/10,K13-P13/U13)</f>
-        <v>3.4410863296610234E-8</v>
+        <v>1.583594260720222E-10</v>
       </c>
     </row>
     <row r="14" spans="2:22">
@@ -2224,7 +2231,7 @@
       </c>
       <c r="C14" s="28">
         <f>1820000*(C13*(C10+273.15))^(-1.5)</f>
-        <v>0.5046674850561782</v>
+        <v>0.49818915002702435</v>
       </c>
       <c r="I14" s="25">
         <f t="shared" ref="I14:I48" si="2">IF(ABS((J14-J13)/J13)&gt;$J$8,1,0)</f>
@@ -2232,64 +2239,64 @@
       </c>
       <c r="J14" s="26">
         <f t="shared" ref="J14:J48" si="3">-LOG(V13*$C$18)</f>
-        <v>7.5058763671885158</v>
+        <v>9.8080731701297701</v>
       </c>
       <c r="K14" s="17">
         <f t="shared" ref="K14:K48" si="4">10^(-J14)/$C$18</f>
-        <v>3.4410863296610195E-8</v>
+        <v>1.5835942607202187E-10</v>
       </c>
       <c r="L14" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105121195915139E-3</v>
+        <v>9.0674469321931666E-5</v>
       </c>
       <c r="M14" s="27">
         <f t="shared" ref="M14:M48" si="5">$C$21/$C$19*L14/K14</f>
-        <v>5.890214320575056E-6</v>
+        <v>1.9960490872156052E-5</v>
       </c>
       <c r="N14" s="27">
         <f t="shared" ref="N14:N48" si="6">$C$23/$C$19^2/M14</f>
-        <v>1.3412505056953103E-3</v>
+        <v>2.2471169547659585E-4</v>
       </c>
       <c r="O14" s="27">
         <f t="shared" ref="O14:O48" si="7">$C$22/$C$18^2/K14</f>
-        <v>2.0310804891667E-7</v>
+        <v>1.8933185367712902E-5</v>
       </c>
       <c r="P14" s="27">
         <f t="shared" ref="P14:P48" si="8">$C$37-2*M14-L14-O14+K14+2*N14</f>
-        <v>3.9765972336194833E-8</v>
+        <v>-1.0508712133892439E-7</v>
       </c>
       <c r="Q14" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.437941060347</v>
+        <v>-119962.15017791292</v>
       </c>
       <c r="R14" s="27">
         <f t="shared" ref="R14:R48" si="9">$C$21/$C$19*(Q14*K14-L14)/K14^2</f>
-        <v>-192.31845543336578</v>
+        <v>-152453.17771626762</v>
       </c>
       <c r="S14" s="27">
         <f t="shared" ref="S14:S48" si="10">$C$23/$C$19^2*(-R14)/M14^2</f>
-        <v>43792.502541632428</v>
+        <v>1716291.0604170358</v>
       </c>
       <c r="T14" s="27">
         <f t="shared" ref="T14:T48" si="11">-$C$22/$C$18^2/K14^2</f>
-        <v>-5.9024397954200154</v>
+        <v>-119558.31008822985</v>
       </c>
       <c r="U14" s="27">
         <f>-2*R14-Q14-T14+1+2*S14</f>
-        <v>100219.98237498736</v>
+        <v>3977009.9365327498</v>
       </c>
       <c r="V14" s="18">
         <f t="shared" ref="V14:V48" si="12">IF((K14-P14/U14)&lt;0,K14/10,K14-P14/U14)</f>
-        <v>3.4410466509747993E-8</v>
-      </c>
-    </row>
-    <row r="15" spans="2:22" ht="25">
+        <v>1.5838584972270818E-10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:22" ht="24">
       <c r="B15" s="7" t="s">
         <v>62</v>
       </c>
       <c r="C15" s="28">
         <f>-1*C14*1^2*(SQRT(C12)/(1+SQRT(C12))-0.3*C12)</f>
-        <v>-4.2571935486603658E-2</v>
+        <v>-7.7170892379409255E-3</v>
       </c>
       <c r="I15" s="25">
         <f t="shared" si="2"/>
@@ -2297,64 +2304,64 @@
       </c>
       <c r="J15" s="26">
         <f t="shared" si="3"/>
-        <v>7.5058813750064486</v>
+        <v>9.8080007103547509</v>
       </c>
       <c r="K15" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509747966E-8</v>
+        <v>1.5838584972270815E-10</v>
       </c>
       <c r="L15" s="27">
         <f t="shared" si="0"/>
-        <v>3.410516977633777E-3</v>
+        <v>9.0671300011027997E-5</v>
       </c>
       <c r="M15" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309034448E-6</v>
+        <v>1.9956463290700118E-5</v>
       </c>
       <c r="N15" s="27">
         <f t="shared" si="6"/>
-        <v>1.34123312942766E-3</v>
+        <v>2.2475704643104352E-4</v>
       </c>
       <c r="O15" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095424163E-7</v>
+        <v>1.8930026727737103E-5</v>
       </c>
       <c r="P15" s="27">
         <f t="shared" si="8"/>
-        <v>3.5292081757010152E-14</v>
+        <v>-2.0722285649574235E-12</v>
       </c>
       <c r="Q15" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923051826</v>
+        <v>-119922.26134952325</v>
       </c>
       <c r="R15" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112222792</v>
+        <v>-152393.53549261737</v>
       </c>
       <c r="S15" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540256584</v>
+        <v>1716312.1758386206</v>
       </c>
       <c r="T15" s="27">
         <f t="shared" si="11"/>
-        <v>-5.90257591819348</v>
+        <v>-119518.42137967872</v>
       </c>
       <c r="U15" s="27">
         <f>-2*R15-Q15-T15+1+2*S15</f>
-        <v>100219.80448172764</v>
+        <v>3976853.1053916779</v>
       </c>
       <c r="V15" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395819E-8</v>
-      </c>
-    </row>
-    <row r="16" spans="2:22" ht="25">
+        <v>1.583858502437806E-10</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22" ht="24">
       <c r="B16" s="7" t="s">
         <v>63</v>
       </c>
       <c r="C16" s="28">
         <f>-1*C14*2^2*(SQRT(C12)/(1+SQRT(C12))-0.3*C12)</f>
-        <v>-0.17028774194641463</v>
+        <v>-3.0868356951763702E-2</v>
       </c>
       <c r="I16" s="25">
         <f t="shared" si="2"/>
@@ -2362,55 +2369,55 @@
       </c>
       <c r="J16" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K16" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L16" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M16" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N16" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O16" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P16" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q16" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R16" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S16" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T16" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U16" s="27">
         <f t="shared" ref="U16:U48" si="13">-2*R16-Q16-T16+1+2*S16</f>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V16" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
+        <v>1.5838585024378063E-10</v>
       </c>
     </row>
     <row r="17" spans="2:22">
@@ -2421,64 +2428,64 @@
       </c>
       <c r="J17" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K17" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L17" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M17" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N17" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O17" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P17" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q17" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R17" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S17" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T17" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U17" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V17" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
-      </c>
-    </row>
-    <row r="18" spans="2:22" ht="23">
+        <v>1.5838585024378063E-10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:22" ht="23.25">
       <c r="B18" s="29" t="s">
         <v>42</v>
       </c>
       <c r="C18" s="30">
         <f>10^(C15)</f>
-        <v>0.90662578084671397</v>
+        <v>0.98238768760753092</v>
       </c>
       <c r="D18" s="15"/>
       <c r="I18" s="25">
@@ -2487,64 +2494,64 @@
       </c>
       <c r="J18" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K18" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L18" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M18" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N18" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O18" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P18" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q18" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R18" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S18" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T18" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U18" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V18" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
-      </c>
-    </row>
-    <row r="19" spans="2:22" ht="23">
+        <v>1.5838585024378063E-10</v>
+      </c>
+    </row>
+    <row r="19" spans="2:22" ht="23.25">
       <c r="B19" s="29" t="s">
         <v>43</v>
       </c>
       <c r="C19" s="30">
         <f>10^(C16)</f>
-        <v>0.67563518476098661</v>
+        <v>0.93139015503435585</v>
       </c>
       <c r="D19" s="15"/>
       <c r="I19" s="25">
@@ -2553,64 +2560,64 @@
       </c>
       <c r="J19" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K19" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L19" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M19" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N19" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O19" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P19" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q19" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R19" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S19" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T19" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U19" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V19" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
-      </c>
-    </row>
-    <row r="20" spans="2:22" ht="25">
+        <v>1.5838585024378063E-10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:22" ht="24">
       <c r="B20" s="7" t="s">
         <v>44</v>
       </c>
       <c r="C20" s="31">
         <f>10^(-1*(356.309-21834.4/(273+C10)-126.834*LOG(273+C10)+0.06092*(273+C10)+1684915/(273+C10)^2))</f>
-        <v>4.0159040551037697E-7</v>
+        <v>3.4343532612165198E-7</v>
       </c>
       <c r="D20" s="15"/>
       <c r="I20" s="25">
@@ -2619,64 +2626,64 @@
       </c>
       <c r="J20" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K20" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L20" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M20" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N20" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O20" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P20" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q20" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R20" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S20" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T20" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U20" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V20" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
-      </c>
-    </row>
-    <row r="21" spans="2:22" ht="25">
+        <v>1.5838585024378063E-10</v>
+      </c>
+    </row>
+    <row r="21" spans="2:22" ht="24">
       <c r="B21" s="7" t="s">
         <v>45</v>
       </c>
       <c r="C21" s="31">
         <f>10^(-1*(107.887-5151.8/(273+C10)-38.926*LOG(273+C10)+0.032528*(273+C10)+563713.9/(273+C10)^2))</f>
-        <v>4.0153122747260345E-11</v>
+        <v>3.2468464988066683E-11</v>
       </c>
       <c r="D21" s="15"/>
       <c r="I21" s="25">
@@ -2685,64 +2692,64 @@
       </c>
       <c r="J21" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K21" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L21" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M21" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N21" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O21" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P21" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q21" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R21" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S21" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T21" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U21" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V21" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
-      </c>
-    </row>
-    <row r="22" spans="2:22" ht="25">
+        <v>1.5838585024378063E-10</v>
+      </c>
+    </row>
+    <row r="22" spans="2:22" ht="24">
       <c r="B22" s="7" t="s">
         <v>46</v>
       </c>
       <c r="C22" s="31">
         <f>10^(-1*(-6.088+4471/(273+C10)+0.01706*(273+C10)))</f>
-        <v>5.7448518257344413E-15</v>
+        <v>2.8935662320507785E-15</v>
       </c>
       <c r="D22" s="15"/>
       <c r="I22" s="25">
@@ -2751,64 +2758,64 @@
       </c>
       <c r="J22" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K22" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L22" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M22" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N22" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O22" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P22" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q22" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R22" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S22" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T22" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U22" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V22" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
-      </c>
-    </row>
-    <row r="23" spans="2:22" ht="25">
+        <v>1.5838585024378063E-10</v>
+      </c>
+    </row>
+    <row r="23" spans="2:22" ht="24">
       <c r="B23" s="7" t="s">
         <v>47</v>
       </c>
       <c r="C23" s="31">
         <f>10^(-1*(171.9065+0.077993*(C10+273)-2839.319/(C10+273)-71.595*LOG10(C10+273)))</f>
-        <v>3.6063303938240078E-9</v>
+        <v>3.8909905853355843E-9</v>
       </c>
       <c r="D23" s="15"/>
       <c r="I23" s="25">
@@ -2817,64 +2824,64 @@
       </c>
       <c r="J23" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K23" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L23" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M23" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N23" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O23" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P23" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q23" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R23" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S23" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T23" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U23" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V23" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
-      </c>
-    </row>
-    <row r="24" spans="2:22" ht="25">
+        <v>1.5838585024378063E-10</v>
+      </c>
+    </row>
+    <row r="24" spans="2:22" ht="24">
       <c r="B24" s="7" t="s">
         <v>48</v>
       </c>
       <c r="C24" s="32">
         <f>-LOG(C20)</f>
-        <v>6.3962166715693991</v>
+        <v>6.4641550348867236</v>
       </c>
       <c r="D24" s="15"/>
       <c r="I24" s="25">
@@ -2883,64 +2890,64 @@
       </c>
       <c r="J24" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K24" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L24" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M24" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N24" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O24" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P24" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q24" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R24" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S24" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T24" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U24" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V24" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
-      </c>
-    </row>
-    <row r="25" spans="2:22" ht="25">
+        <v>1.5838585024378063E-10</v>
+      </c>
+    </row>
+    <row r="25" spans="2:22" ht="24">
       <c r="B25" s="7" t="s">
         <v>49</v>
       </c>
       <c r="C25" s="32">
         <f>-LOG(C21)</f>
-        <v>10.39628067356921</v>
+        <v>10.488538243033087</v>
       </c>
       <c r="D25" s="15"/>
       <c r="I25" s="25">
@@ -2949,64 +2956,64 @@
       </c>
       <c r="J25" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K25" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L25" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M25" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N25" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O25" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P25" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q25" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R25" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S25" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T25" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U25" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V25" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
-      </c>
-    </row>
-    <row r="26" spans="2:22" ht="25">
+        <v>1.5838585024378063E-10</v>
+      </c>
+    </row>
+    <row r="26" spans="2:22" ht="24">
       <c r="B26" s="7" t="s">
         <v>50</v>
       </c>
       <c r="C26" s="32">
         <f>-LOG(C22)</f>
-        <v>14.240721168384882</v>
+        <v>14.538566572438164</v>
       </c>
       <c r="D26" s="15"/>
       <c r="I26" s="25">
@@ -3015,64 +3022,64 @@
       </c>
       <c r="J26" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K26" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L26" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M26" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N26" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O26" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P26" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q26" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R26" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S26" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T26" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U26" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V26" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
-      </c>
-    </row>
-    <row r="27" spans="2:22" ht="25">
+        <v>1.5838585024378063E-10</v>
+      </c>
+    </row>
+    <row r="27" spans="2:22" ht="24">
       <c r="B27" s="7" t="s">
         <v>51</v>
       </c>
       <c r="C27" s="32">
         <f>-LOG(C23)</f>
-        <v>8.4429344879182242</v>
+        <v>8.4099398200165485</v>
       </c>
       <c r="D27" s="33"/>
       <c r="F27" s="34"/>
@@ -3082,64 +3089,64 @@
       </c>
       <c r="J27" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K27" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L27" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M27" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N27" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O27" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P27" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q27" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R27" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S27" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T27" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U27" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V27" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
-      </c>
-    </row>
-    <row r="28" spans="2:22" ht="24">
+        <v>1.5838585024378063E-10</v>
+      </c>
+    </row>
+    <row r="28" spans="2:22" ht="23.25">
       <c r="B28" s="35" t="s">
         <v>52</v>
       </c>
       <c r="C28" s="36">
         <f>10^(-C6)/C18</f>
-        <v>9.1742788333889117E-9</v>
+        <v>1.0179280671110216E-10</v>
       </c>
       <c r="D28" s="15" t="s">
         <v>8</v>
@@ -3151,64 +3158,64 @@
       </c>
       <c r="J28" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K28" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L28" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M28" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N28" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O28" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P28" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q28" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R28" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S28" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T28" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U28" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V28" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
-      </c>
-    </row>
-    <row r="29" spans="2:22" ht="24">
+        <v>1.5838585024378063E-10</v>
+      </c>
+    </row>
+    <row r="29" spans="2:22" ht="23.25">
       <c r="B29" s="35" t="s">
         <v>53</v>
       </c>
       <c r="C29" s="37">
         <f>C22/C28/C18^2</f>
-        <v>7.6181718831964212E-7</v>
+        <v>2.9454422816491705E-5</v>
       </c>
       <c r="D29" s="15" t="s">
         <v>8</v>
@@ -3219,55 +3226,55 @@
       </c>
       <c r="J29" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K29" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L29" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M29" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N29" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O29" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P29" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q29" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R29" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S29" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T29" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U29" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V29" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
+        <v>1.5838585024378063E-10</v>
       </c>
     </row>
     <row r="30" spans="2:22">
@@ -3280,55 +3287,55 @@
       </c>
       <c r="J30" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K30" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L30" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M30" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N30" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O30" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P30" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q30" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R30" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S30" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T30" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U30" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V30" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
+        <v>1.5838585024378063E-10</v>
       </c>
     </row>
     <row r="31" spans="2:22">
@@ -3341,64 +3348,64 @@
       </c>
       <c r="J31" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K31" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L31" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M31" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N31" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O31" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P31" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q31" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R31" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S31" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T31" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U31" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V31" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
-      </c>
-    </row>
-    <row r="32" spans="2:22" ht="25">
+        <v>1.5838585024378063E-10</v>
+      </c>
+    </row>
+    <row r="32" spans="2:22" ht="24">
       <c r="B32" s="35" t="s">
         <v>54</v>
       </c>
       <c r="C32" s="36">
         <f>SUM(C33:C35)</f>
-        <v>3.8453799870987143E-3</v>
+        <v>1.3591107173834457E-4</v>
       </c>
       <c r="D32" s="15" t="s">
         <v>8</v>
@@ -3409,64 +3416,64 @@
       </c>
       <c r="J32" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K32" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L32" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M32" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N32" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O32" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P32" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q32" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R32" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S32" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T32" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U32" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V32" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
-      </c>
-    </row>
-    <row r="33" spans="2:22" ht="25">
+        <v>1.5838585024378063E-10</v>
+      </c>
+    </row>
+    <row r="33" spans="2:22" ht="24">
       <c r="B33" s="35" t="s">
         <v>55</v>
       </c>
       <c r="C33" s="31">
         <f>C18^2*C28/C20*(C7/50000-C22/(C18)^2/C28+C28)/(1+2*C21/C19/C28)</f>
-        <v>7.04290449515074E-5</v>
+        <v>2.8953301385418117E-8</v>
       </c>
       <c r="D33" s="15" t="s">
         <v>8</v>
@@ -3477,64 +3484,64 @@
       </c>
       <c r="J33" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K33" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L33" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M33" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N33" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O33" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P33" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q33" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R33" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S33" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T33" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U33" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V33" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
-      </c>
-    </row>
-    <row r="34" spans="2:22" ht="26">
+        <v>1.5838585024378063E-10</v>
+      </c>
+    </row>
+    <row r="34" spans="2:22" ht="24.75">
       <c r="B34" s="35" t="s">
         <v>56</v>
       </c>
       <c r="C34" s="36">
         <f>(C7/50000-C22/(C18)^2/C28+C28)/(1+2*C21/C19/C28)</f>
-        <v>3.7506545272039012E-3</v>
+        <v>1.012185578976033E-4</v>
       </c>
       <c r="D34" s="15" t="s">
         <v>8</v>
@@ -3545,64 +3552,64 @@
       </c>
       <c r="J34" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K34" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L34" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M34" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N34" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O34" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P34" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q34" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R34" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S34" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T34" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U34" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V34" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
-      </c>
-    </row>
-    <row r="35" spans="2:22" ht="26">
+        <v>1.5838585024378063E-10</v>
+      </c>
+    </row>
+    <row r="35" spans="2:22" ht="24.75">
       <c r="B35" s="35" t="s">
         <v>60</v>
       </c>
       <c r="C35" s="37">
         <f>C21/C19/C28*(C7/50000-C22/(C18)^2/C28+C28)/(1+2*C21/C19/C28)</f>
-        <v>2.4296414943306097E-5</v>
+        <v>3.4663560539355861E-5</v>
       </c>
       <c r="D35" s="15" t="s">
         <v>8</v>
@@ -3614,55 +3621,55 @@
       </c>
       <c r="J35" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K35" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L35" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M35" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N35" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O35" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P35" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q35" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R35" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S35" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T35" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U35" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V35" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
+        <v>1.5838585024378063E-10</v>
       </c>
     </row>
     <row r="36" spans="2:22">
@@ -3671,7 +3678,7 @@
       </c>
       <c r="C36" s="36">
         <f>2*C33+C34+C28-C22/C28/C18^2</f>
-        <v>3.8907599741974299E-3</v>
+        <v>7.1822143476689139E-5</v>
       </c>
       <c r="D36" s="15" t="s">
         <v>31</v>
@@ -3682,55 +3689,55 @@
       </c>
       <c r="J36" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K36" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L36" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M36" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N36" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O36" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P36" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q36" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R36" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S36" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T36" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U36" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V36" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
+        <v>1.5838585024378063E-10</v>
       </c>
     </row>
     <row r="37" spans="2:22">
@@ -3739,7 +3746,7 @@
       </c>
       <c r="C37" s="36">
         <f>C7/50000-2*C8/100000</f>
-        <v>7.4000000000000021E-4</v>
+        <v>-3.0000000000000003E-4</v>
       </c>
       <c r="D37" s="15" t="s">
         <v>31</v>
@@ -3750,55 +3757,55 @@
       </c>
       <c r="J37" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K37" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L37" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M37" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N37" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O37" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P37" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q37" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R37" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S37" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T37" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U37" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V37" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
+        <v>1.5838585024378063E-10</v>
       </c>
     </row>
     <row r="38" spans="2:22">
@@ -3811,64 +3818,64 @@
       </c>
       <c r="J38" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K38" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L38" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M38" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N38" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O38" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P38" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q38" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R38" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S38" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T38" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U38" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V38" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
-      </c>
-    </row>
-    <row r="39" spans="2:22" ht="23">
+        <v>1.5838585024378063E-10</v>
+      </c>
+    </row>
+    <row r="39" spans="2:22" ht="23.25">
       <c r="B39" s="29" t="s">
         <v>65</v>
       </c>
       <c r="C39" s="31">
         <f>C28/(C28+C20)</f>
-        <v>2.2334633874491087E-2</v>
+        <v>2.9630802932922293E-4</v>
       </c>
       <c r="D39" s="38"/>
       <c r="I39" s="25">
@@ -3877,64 +3884,64 @@
       </c>
       <c r="J39" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K39" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L39" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M39" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N39" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O39" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P39" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q39" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R39" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S39" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T39" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U39" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V39" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
-      </c>
-    </row>
-    <row r="40" spans="2:22" ht="23">
+        <v>1.5838585024378063E-10</v>
+      </c>
+    </row>
+    <row r="40" spans="2:22" ht="23.25">
       <c r="B40" s="29" t="s">
         <v>57</v>
       </c>
       <c r="C40" s="31">
         <f>1-C39</f>
-        <v>0.97766536612550892</v>
+        <v>0.99970369197067077</v>
       </c>
       <c r="I40" s="25">
         <f t="shared" si="2"/>
@@ -3942,64 +3949,64 @@
       </c>
       <c r="J40" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K40" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L40" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M40" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N40" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O40" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P40" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q40" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R40" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S40" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T40" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U40" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V40" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
-      </c>
-    </row>
-    <row r="41" spans="2:22" ht="23">
+        <v>1.5838585024378063E-10</v>
+      </c>
+    </row>
+    <row r="41" spans="2:22" ht="23.25">
       <c r="B41" s="29" t="s">
         <v>58</v>
       </c>
       <c r="C41" s="31">
         <f>1-C28/(C28+C21)</f>
-        <v>4.3576340829691862E-3</v>
+        <v>0.2418304592020909</v>
       </c>
       <c r="I41" s="25">
         <f t="shared" si="2"/>
@@ -4007,55 +4014,55 @@
       </c>
       <c r="J41" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K41" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L41" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M41" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N41" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O41" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P41" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q41" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R41" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S41" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T41" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U41" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V41" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
+        <v>1.5838585024378063E-10</v>
       </c>
     </row>
     <row r="42" spans="2:22">
@@ -4066,64 +4073,64 @@
       </c>
       <c r="J42" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K42" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L42" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M42" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N42" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O42" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P42" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q42" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R42" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S42" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T42" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U42" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V42" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
-      </c>
-    </row>
-    <row r="43" spans="2:22" ht="25">
+        <v>1.5838585024378063E-10</v>
+      </c>
+    </row>
+    <row r="43" spans="2:22" ht="24">
       <c r="B43" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C43" s="39">
         <f>50000*(C34+2*C35+C29-C28)</f>
-        <v>189.99999999999997</v>
+        <v>10.000000000000002</v>
       </c>
       <c r="D43" s="15" t="s">
         <v>40</v>
@@ -4134,55 +4141,55 @@
       </c>
       <c r="J43" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K43" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L43" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M43" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N43" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O43" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P43" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q43" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R43" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S43" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T43" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U43" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V43" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
+        <v>1.5838585024378063E-10</v>
       </c>
     </row>
     <row r="44" spans="2:22">
@@ -4191,7 +4198,7 @@
       </c>
       <c r="C44" s="44">
         <f>C19^2*C8/2.5/40000*C35/C23</f>
-        <v>4.705357558019065</v>
+        <v>1.9320407621494822</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -4201,55 +4208,55 @@
       </c>
       <c r="J44" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K44" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L44" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M44" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N44" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O44" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P44" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q44" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R44" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S44" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T44" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U44" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V44" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
+        <v>1.5838585024378063E-10</v>
       </c>
     </row>
     <row r="45" spans="2:22">
@@ -4259,55 +4266,55 @@
       </c>
       <c r="J45" s="26">
         <f>-LOG(V44*$C$18)</f>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K45" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L45" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M45" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N45" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O45" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P45" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q45" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R45" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S45" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T45" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U45" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V45" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
+        <v>1.5838585024378063E-10</v>
       </c>
     </row>
     <row r="46" spans="2:22">
@@ -4316,7 +4323,7 @@
       </c>
       <c r="C46" s="32">
         <f>LOG(C44)</f>
-        <v>0.67259263086092791</v>
+        <v>0.28601628491065617</v>
       </c>
       <c r="D46" s="15"/>
       <c r="I46" s="25">
@@ -4325,64 +4332,64 @@
       </c>
       <c r="J46" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K46" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L46" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M46" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N46" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O46" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P46" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q46" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R46" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S46" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T46" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U46" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V46" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
-      </c>
-    </row>
-    <row r="47" spans="2:22" ht="25">
+        <v>1.5838585024378063E-10</v>
+      </c>
+    </row>
+    <row r="47" spans="2:22" ht="24">
       <c r="B47" s="35" t="s">
         <v>59</v>
       </c>
       <c r="C47" s="32">
         <f>C6-C46</f>
-        <v>7.4074073691390723</v>
+        <v>9.7139837150893431</v>
       </c>
       <c r="I47" s="25">
         <f t="shared" si="2"/>
@@ -4390,64 +4397,64 @@
       </c>
       <c r="J47" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K47" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L47" s="27">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M47" s="27">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N47" s="27">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O47" s="27">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P47" s="27">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q47" s="27">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R47" s="27">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S47" s="27">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T47" s="27">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U47" s="27">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V47" s="18">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
-      </c>
-    </row>
-    <row r="48" spans="2:22" ht="26" thickBot="1">
+        <v>1.5838585024378063E-10</v>
+      </c>
+    </row>
+    <row r="48" spans="2:22" ht="24.75" thickBot="1">
       <c r="B48" s="7" t="s">
         <v>36</v>
       </c>
       <c r="C48" s="32">
         <f>C8-100000*N48</f>
-        <v>18.876687058776412</v>
+        <v>2.5242952674633941</v>
       </c>
       <c r="D48" s="15" t="s">
         <v>40</v>
@@ -4458,55 +4465,55 @@
       </c>
       <c r="J48" s="26">
         <f t="shared" si="3"/>
-        <v>7.505881375010893</v>
+        <v>9.8080007089259684</v>
       </c>
       <c r="K48" s="17">
         <f t="shared" si="4"/>
-        <v>3.4410466509395759E-8</v>
+        <v>1.5838585024378034E-10</v>
       </c>
       <c r="L48" s="41">
         <f t="shared" si="0"/>
-        <v>3.4105169776380896E-3</v>
+        <v>9.0671299948539842E-5</v>
       </c>
       <c r="M48" s="41">
         <f t="shared" si="5"/>
-        <v>5.8902906309711828E-6</v>
+        <v>1.9956463211292087E-5</v>
       </c>
       <c r="N48" s="41">
         <f t="shared" si="6"/>
-        <v>1.3412331294122358E-3</v>
+        <v>2.2475704732536605E-4</v>
       </c>
       <c r="O48" s="41">
         <f t="shared" si="7"/>
-        <v>2.0311039095632054E-7</v>
+        <v>1.8930026665459378E-5</v>
       </c>
       <c r="P48" s="41">
         <f t="shared" si="8"/>
-        <v>-7.3725747729014302E-18</v>
+        <v>-1.0842021724855044E-18</v>
       </c>
       <c r="Q48" s="41">
         <f t="shared" si="1"/>
-        <v>-12243.472923082876</v>
+        <v>-119922.26056311571</v>
       </c>
       <c r="R48" s="41">
         <f t="shared" si="9"/>
-        <v>-192.32295112621858</v>
+        <v>-152393.53431681532</v>
       </c>
       <c r="S48" s="41">
         <f t="shared" si="10"/>
-        <v>43792.391540158045</v>
+        <v>1716312.1762549342</v>
       </c>
       <c r="T48" s="41">
         <f t="shared" si="11"/>
-        <v>-5.9025759183143123</v>
+        <v>-119518.42059327355</v>
       </c>
       <c r="U48" s="41">
         <f t="shared" si="13"/>
-        <v>100219.80448156972</v>
+        <v>3976853.1022998882</v>
       </c>
       <c r="V48" s="42">
         <f t="shared" si="12"/>
-        <v>3.4410466509395832E-8</v>
+        <v>1.5838585024378063E-10</v>
       </c>
     </row>
     <row r="49" spans="2:14">
@@ -4515,7 +4522,7 @@
       </c>
       <c r="C49" s="40">
         <f>C6+LOG(C7*C8)</f>
-        <v>12.543445031770428</v>
+        <v>12.397940008672037</v>
       </c>
       <c r="D49" s="15"/>
       <c r="J49" s="26"/>
@@ -4526,7 +4533,7 @@
       </c>
       <c r="C50" s="40">
         <f>2*C47-C6</f>
-        <v>6.7348147382781445</v>
+        <v>9.4279674301786862</v>
       </c>
       <c r="D50" s="15"/>
       <c r="M50" s="43"/>
@@ -4540,10 +4547,42 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
+  <customProperties>
+    <customPr name="SSC_SHEET_GUID" r:id="rId1"/>
+  </customProperties>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC1814EC-D66A-43B0-BA3D-94765F2A1F23}">
+  <dimension ref="C1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="3:5">
+      <c r="C1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="3:5">
+      <c r="C2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>